<commit_message>
inclusão de orcamento do transporte
</commit_message>
<xml_diff>
--- a/PastaDocsAdministrativos/Orcamento.xlsx
+++ b/PastaDocsAdministrativos/Orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Downloads\GITexercicio\3SIPG-ExemploGit-2024\PastaDocsAdministrativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E36F9F-DFEC-46F7-89A4-1821C095E67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B84DFC-8EEB-4883-8CD6-C888C2FD720C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Item de gasto</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t xml:space="preserve">PREVISÂO ORÇAMENTÁRIA - PROJETO EXEMPLO </t>
+  </si>
+  <si>
+    <t>Pessoal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telecom </t>
+  </si>
+  <si>
+    <t>Refeições</t>
+  </si>
+  <si>
+    <t>Transporte</t>
   </si>
 </sst>
 </file>
@@ -65,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -231,11 +243,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -243,34 +281,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -553,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:E6"/>
+  <dimension ref="B1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,51 +610,67 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
+      <c r="B5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D6:E6"/>
     <mergeCell ref="D5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>